<commit_message>
Fixed a mergeconflict between peter and i
</commit_message>
<xml_diff>
--- a/files/assesments/firstround/assesments-ahmet.xlsx
+++ b/files/assesments/firstround/assesments-ahmet.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
   <si>
     <t>Self assesment</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>Active collaborator, motivated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Very motivated. Asking everyone where we are in the project, and what needs to be done. </t>
   </si>
 </sst>
 </file>
@@ -564,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -731,8 +734,12 @@
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="4"/>
+      <c r="B21" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="22" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">

</xml_diff>

<commit_message>
Finished my assesments review - peter
</commit_message>
<xml_diff>
--- a/files/assesments/firstround/assesments-ahmet.xlsx
+++ b/files/assesments/firstround/assesments-ahmet.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lanes\OneDrive\Dokumenter\uni\2. semester\epic\files\assesments\firstround\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Piiit\Documents\Honeyjar\files\assesments\firstround\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D661C323-A592-4CEB-BAFC-7B12323D9FC1}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7536" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Peer  and self assessment" sheetId="2" r:id="rId1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
   <si>
     <t>Self assesment</t>
   </si>
@@ -114,12 +115,15 @@
   </si>
   <si>
     <t xml:space="preserve">Very motivated. Asking everyone where we are in the project, and what needs to be done. </t>
+  </si>
+  <si>
+    <t>Very good research, sharing relevant information with everyone.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -293,10 +297,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:A5" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
-  <autoFilter ref="A1:A5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:A5" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
+  <autoFilter ref="A1:A5" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Grade" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Grade" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -564,22 +568,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.125" customWidth="1"/>
-    <col min="2" max="2" width="21.625" customWidth="1"/>
-    <col min="3" max="3" width="64.75" customWidth="1"/>
+    <col min="1" max="1" width="40.09765625" customWidth="1"/>
+    <col min="2" max="2" width="21.59765625" customWidth="1"/>
+    <col min="3" max="3" width="64.69921875" customWidth="1"/>
     <col min="7" max="7" width="54" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>8</v>
       </c>
@@ -590,21 +594,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="7"/>
     </row>
-    <row r="3" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
@@ -615,7 +619,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
@@ -626,50 +630,54 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="4"/>
     </row>
-    <row r="13" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>9</v>
       </c>
@@ -680,21 +688,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
@@ -705,7 +713,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
@@ -716,21 +724,21 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
@@ -741,50 +749,50 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="6"/>
       <c r="C23" s="4"/>
     </row>
-    <row r="24" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="4"/>
     </row>
-    <row r="25" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
     </row>
-    <row r="27" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="9"/>
     </row>
-    <row r="28" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="9"/>
     </row>
-    <row r="29" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>13</v>
       </c>
@@ -798,14 +806,14 @@
     <mergeCell ref="B29:C29"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Give at least two examples" sqref="C2:C11 C15:C24"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Give at least two examples" sqref="C2:C11 C15:C24" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please choose a grade">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please choose a grade" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>Sheet1!$A$2:$A$5</xm:f>
           </x14:formula1>
@@ -818,19 +826,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="10.875" customWidth="1"/>
+    <col min="3" max="3" width="10.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -841,7 +849,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -852,7 +860,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -863,7 +871,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -874,7 +882,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -885,7 +893,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -894,7 +902,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -903,7 +911,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -912,7 +920,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -921,7 +929,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -930,7 +938,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -939,7 +947,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -948,7 +956,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -957,7 +965,7 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -966,7 +974,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -975,7 +983,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -984,7 +992,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -993,7 +1001,7 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1002,7 +1010,7 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1011,7 +1019,7 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1020,7 +1028,7 @@
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1029,7 +1037,7 @@
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1038,7 +1046,7 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>

</xml_diff>

<commit_message>
Daniels assesments merged in to my structure
</commit_message>
<xml_diff>
--- a/files/assesments/firstround/assesments-ahmet.xlsx
+++ b/files/assesments/firstround/assesments-ahmet.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Piiit\Documents\Honeyjar\files\assesments\firstround\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lanes\OneDrive\Dokumenter\uni\2. semester\epic\files\assesments\firstround\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D661C323-A592-4CEB-BAFC-7B12323D9FC1}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7536" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Peer  and self assessment" sheetId="2" r:id="rId1"/>
@@ -19,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$A$5</definedName>
   </definedNames>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
   <si>
     <t>Self assesment</t>
   </si>
@@ -118,12 +117,18 @@
   </si>
   <si>
     <t>Very good research, sharing relevant information with everyone.</t>
+  </si>
+  <si>
+    <t>Has done extremely well in working with the group, both posting relevant articles with excellent comments and asking relevant questions to other group members.</t>
+  </si>
+  <si>
+    <t>Very active on discord, providing tons upon tons of sources.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -297,10 +302,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:A5" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
-  <autoFilter ref="A1:A5" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:A5" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
+  <autoFilter ref="A1:A5"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Grade" dataDxfId="0"/>
+    <tableColumn id="1" name="Grade" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -568,22 +573,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C11" activeCellId="1" sqref="C9 C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.09765625" customWidth="1"/>
-    <col min="2" max="2" width="21.59765625" customWidth="1"/>
-    <col min="3" max="3" width="64.69921875" customWidth="1"/>
+    <col min="1" max="1" width="40.125" customWidth="1"/>
+    <col min="2" max="2" width="21.625" customWidth="1"/>
+    <col min="3" max="3" width="64.75" customWidth="1"/>
     <col min="7" max="7" width="54" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>8</v>
       </c>
@@ -594,21 +599,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="7"/>
     </row>
-    <row r="3" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
@@ -619,7 +624,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
@@ -630,21 +635,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
@@ -655,29 +660,33 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="4"/>
     </row>
-    <row r="13" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>9</v>
       </c>
@@ -688,21 +697,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
@@ -713,7 +722,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
@@ -724,21 +733,21 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
@@ -749,50 +758,54 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="4"/>
-    </row>
-    <row r="23" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="6"/>
       <c r="C23" s="4"/>
     </row>
-    <row r="24" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="4"/>
     </row>
-    <row r="25" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
     </row>
-    <row r="27" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="9"/>
     </row>
-    <row r="28" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="9"/>
     </row>
-    <row r="29" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>13</v>
       </c>
@@ -806,14 +819,14 @@
     <mergeCell ref="B29:C29"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Give at least two examples" sqref="C2:C11 C15:C24" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Give at least two examples" sqref="C2:C11 C15:C24"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please choose a grade" xr:uid="{00000000-0002-0000-0000-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please choose a grade">
           <x14:formula1>
             <xm:f>Sheet1!$A$2:$A$5</xm:f>
           </x14:formula1>
@@ -826,19 +839,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.8984375" customWidth="1"/>
+    <col min="3" max="3" width="10.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -849,7 +862,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -860,7 +873,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -871,7 +884,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -882,7 +895,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -893,7 +906,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -902,7 +915,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -911,7 +924,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -920,7 +933,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -929,7 +942,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -938,7 +951,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -947,7 +960,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -956,7 +969,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -965,7 +978,7 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -974,7 +987,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -983,7 +996,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -992,7 +1005,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1001,7 +1014,7 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1010,7 +1023,7 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1019,7 +1032,7 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1028,7 +1041,7 @@
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1037,7 +1050,7 @@
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1046,7 +1059,7 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>

</xml_diff>

<commit_message>
merged jacobs comments into the structure
</commit_message>
<xml_diff>
--- a/files/assesments/firstround/assesments-ahmet.xlsx
+++ b/files/assesments/firstround/assesments-ahmet.xlsx
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$A$5</definedName>
   </definedNames>
-  <calcPr calcId="150000" iterateDelta="1E-4"/>
+  <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
   <si>
     <t>Self assesment</t>
   </si>
@@ -123,6 +123,18 @@
   </si>
   <si>
     <t>Very active on discord, providing tons upon tons of sources.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Been very consistant, active and respectful in his use of Discord and GitHub. Has uploaded many relevant research articles, and made really good explanations of his research within machine learning. 
+2) Ahmet has been very reflective of his research and included all
+other members of the project in his research in a very respectful and 
+teaching kind of way.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Been very informative and respectful on Discord text chat as well as
+in meetings. 
+2) Actively collaborating at a high level of interaction with the project group as well as a with each individual member. </t>
   </si>
 </sst>
 </file>
@@ -576,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C11" activeCellId="1" sqref="C9 C11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -610,8 +622,12 @@
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="4"/>
+      <c r="B3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="4" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -708,8 +724,12 @@
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="4"/>
+      <c r="B16" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="17" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">

</xml_diff>